<commit_message>
editign gantt chart bc project management
</commit_message>
<xml_diff>
--- a/Report/ganttChart.xlsx
+++ b/Report/ganttChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46c66270056a4b13/Documents/UWE_CS_Y2/SD/GroupProject/systems-development-group-work/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="8_{BD0E18E2-C511-4D01-B55E-1AD603F7CB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B3B5EBA-3FC6-4288-A290-704E4246B20A}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{BD0E18E2-C511-4D01-B55E-1AD603F7CB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1C2B086-4284-457A-A245-A41B0D44E393}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0770252E-A40D-4073-814B-41740F9415ED}"/>
   </bookViews>
@@ -267,7 +267,7 @@
                   <c:v>45358</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45365</c:v>
+                  <c:v>45372</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -354,10 +354,10 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>7</c:v>
@@ -1134,9 +1134,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1174,7 +1174,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1280,7 +1280,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1422,7 +1422,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1433,7 +1433,7 @@
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="133" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1553,11 +1553,11 @@
         <v>45358</v>
       </c>
       <c r="D9" s="1">
-        <v>45365</v>
+        <v>45372</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
@@ -1568,11 +1568,11 @@
         <v>45358</v>
       </c>
       <c r="D10" s="1">
-        <v>45365</v>
+        <v>45372</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
@@ -1580,10 +1580,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1">
-        <v>45365</v>
+        <v>45372</v>
       </c>
       <c r="D11" s="1">
-        <v>45372</v>
+        <v>45379</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>

</xml_diff>